<commit_message>
Draft grid battery edits and fix to battery cost calculation
</commit_message>
<xml_diff>
--- a/InputData/elec/GBCGpUNR/Grid Bat Cap Growth per Unit Net Revenue.xlsx
+++ b/InputData/elec/GBCGpUNR/Grid Bat Cap Growth per Unit Net Revenue.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\elec\GBCGpUNR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22FBC464-409D-476B-849A-6B925C9C0E25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BDD170D-E14C-4316-A804-4B5CF355D36C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-80" yWindow="-80" windowWidth="19360" windowHeight="10360" activeTab="1" xr2:uid="{7E47E401-4FF2-4F75-986A-BA871D3584BD}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{7E47E401-4FF2-4F75-986A-BA871D3584BD}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -428,18 +428,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1BF9ED0-8E48-4355-BDAD-C352BC3B92D2}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A10" sqref="A10:H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -447,7 +447,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
@@ -464,16 +464,16 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="62.85546875" customWidth="1"/>
+    <col min="1" max="1" width="62.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -481,12 +481,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>
       <c r="B2">
-        <v>2000</v>
+        <v>750</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Calibrate battery storage deployment
</commit_message>
<xml_diff>
--- a/InputData/elec/GBCGpUNR/Grid Bat Cap Growth per Unit Net Revenue.xlsx
+++ b/InputData/elec/GBCGpUNR/Grid Bat Cap Growth per Unit Net Revenue.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\elec\GBCGpUNR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BDD170D-E14C-4316-A804-4B5CF355D36C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C74A81D-3725-4C8A-8875-8C49E5853CD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{7E47E401-4FF2-4F75-986A-BA871D3584BD}"/>
+    <workbookView xWindow="-24120" yWindow="-1185" windowWidth="24240" windowHeight="13140" xr2:uid="{7E47E401-4FF2-4F75-986A-BA871D3584BD}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -486,7 +486,7 @@
         <v>6</v>
       </c>
       <c r="B2">
-        <v>750</v>
+        <v>2000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>